<commit_message>
update inventory analysis Excel
</commit_message>
<xml_diff>
--- a/diseño/AnálisisInvetario.xlsx
+++ b/diseño/AnálisisInvetario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juane\OneDrive\Mision TIC 2021\Ciclo 3\Desarrollo de Software\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/af6ca4d8c979caca/Mision TIC 2021/Ciclo 3/Desarrollo de Software/ProyectoTransversal/diseño/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92627531-9AE7-46D7-BF2B-813186A245E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{92627531-9AE7-46D7-BF2B-813186A245E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7DDE8533-1CD0-4341-9845-5C965E79ABA7}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-27150" yWindow="735" windowWidth="25800" windowHeight="12570" tabRatio="574" xr2:uid="{EB208667-042A-4012-A5A0-AE712C88FEDD}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="574" xr2:uid="{EB208667-042A-4012-A5A0-AE712C88FEDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
   <si>
     <t>ID</t>
   </si>
@@ -162,9 +162,6 @@
     <t>ID bill</t>
   </si>
   <si>
-    <t>Lote</t>
-  </si>
-  <si>
     <t>Bill Order Items</t>
   </si>
   <si>
@@ -181,6 +178,12 @@
   </si>
   <si>
     <t>Date entry</t>
+  </si>
+  <si>
+    <t>Storage</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -275,7 +278,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -348,32 +351,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -410,6 +393,19 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -428,25 +424,9 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -765,13 +745,16 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.28515625" bestFit="1" customWidth="1"/>
@@ -779,14 +762,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
+      <c r="A1" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
       <c r="G1" s="2"/>
       <c r="I1" s="1" t="s">
         <v>10</v>
@@ -834,14 +817,14 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I4" s="40" t="s">
+      <c r="I4" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="40"/>
-      <c r="L4" s="41" t="s">
+      <c r="J4" s="35"/>
+      <c r="L4" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="41"/>
+      <c r="M4" s="36"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I5" s="19" t="s">
@@ -858,13 +841,13 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
       <c r="F6" s="6"/>
       <c r="I6" s="20">
         <v>1</v>
@@ -948,23 +931,23 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
       <c r="G12" s="24"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="39" t="s">
+      <c r="I12" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="J12" s="39"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="39"/>
-      <c r="M12" s="39"/>
+      <c r="J12" s="44"/>
+      <c r="K12" s="44"/>
+      <c r="L12" s="44"/>
+      <c r="M12" s="44"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
@@ -1108,8 +1091,8 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="44" t="s">
-        <v>41</v>
+      <c r="A20" s="45" t="s">
+        <v>47</v>
       </c>
       <c r="B20" s="45"/>
       <c r="C20" s="45"/>
@@ -1117,12 +1100,12 @@
       <c r="E20" s="45"/>
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
-      <c r="I20" s="42" t="s">
+      <c r="I20" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="J20" s="42"/>
-      <c r="K20" s="42"/>
-      <c r="L20" s="42"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
       <c r="M20" s="15"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -1133,10 +1116,10 @@
         <v>36</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E21" s="21" t="s">
         <v>3</v>
@@ -1153,7 +1136,7 @@
         <v>34</v>
       </c>
       <c r="L21" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -1166,7 +1149,7 @@
       <c r="C22" s="23">
         <v>1</v>
       </c>
-      <c r="D22" s="46">
+      <c r="D22" s="34">
         <v>44459</v>
       </c>
       <c r="E22" s="23"/>
@@ -1191,7 +1174,7 @@
       <c r="C23" s="23">
         <v>1</v>
       </c>
-      <c r="D23" s="46">
+      <c r="D23" s="34">
         <v>44459</v>
       </c>
       <c r="E23" s="23"/>
@@ -1215,10 +1198,10 @@
       <c r="J25" s="26"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="34" t="s">
+      <c r="A26" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="34"/>
+      <c r="B26" s="39"/>
       <c r="C26" s="24"/>
       <c r="D26" s="24"/>
       <c r="E26" s="24"/>
@@ -1287,13 +1270,16 @@
       <c r="G31" s="14"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="37"/>
+      <c r="A32" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="41"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="42"/>
+      <c r="G32" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="30" t="s">
@@ -1303,7 +1289,7 @@
         <v>6</v>
       </c>
       <c r="C33" s="30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D33" s="30" t="s">
         <v>40</v>
@@ -1389,16 +1375,16 @@
     </filterColumn>
   </autoFilter>
   <mergeCells count="10">
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="I12:M12"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="L4:M4"/>
     <mergeCell ref="I20:L20"/>
     <mergeCell ref="A6:E6"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="I12:M12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" xr:uid="{6E99CEEF-72B6-4D72-84C7-FC3FAFF0CFE5}"/>

</xml_diff>